<commit_message>
CUP and OUP Added
</commit_message>
<xml_diff>
--- a/list of packages.xlsx
+++ b/list of packages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco\Documents\Proyectos\Academic Journal Packages\academic-journal-packages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9DEBC7-6C34-4053-9870-0181DE00AD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E38741-A9DB-4DD5-A51F-6041C130C8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="1200" windowWidth="22125" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="2100" windowWidth="22125" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -69,18 +69,12 @@
     <t>http://metadata.springernature.com/metadata/kbart/Springer_Global_Complete_Journals_2021-06-01.txt</t>
   </si>
   <si>
-    <t>SPRINGER</t>
-  </si>
-  <si>
     <t>Springer</t>
   </si>
   <si>
     <t>Nature</t>
   </si>
   <si>
-    <t>NATURE</t>
-  </si>
-  <si>
     <t>http://metadata.springernature.com/metadata/kbart/SpringerNature_Global_Nature-Com_AllTitles_2021_2021-06-01.txt</t>
   </si>
   <si>
@@ -109,6 +103,39 @@
   </si>
   <si>
     <t>kbart</t>
+  </si>
+  <si>
+    <t>CUP_FP</t>
+  </si>
+  <si>
+    <t>Cambridge Journals Full Package</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/services/aop-cambridge-core/kbart/create/bespoke/BE6D264D98C2E9F9BFDC17C422C3C696</t>
+  </si>
+  <si>
+    <t>OUP_CC</t>
+  </si>
+  <si>
+    <t>Oxford Current Collection</t>
+  </si>
+  <si>
+    <t>http://fdslive.oup.com/www.oup.com/academic/content/librarian/OxfordUniversityPress_Global_2021JournalsCurrentCollection.zip</t>
+  </si>
+  <si>
+    <t>OUP_OA</t>
+  </si>
+  <si>
+    <t>Oxford Open Access Tiles</t>
+  </si>
+  <si>
+    <t>http://fdslive.oup.com/www.oup.com/academic/content/librarian/OxfordUniversityPress_Global_2021JournalsOpenAccess.zip</t>
+  </si>
+  <si>
+    <t>SN_SPRINGER</t>
+  </si>
+  <si>
+    <t>SN_NATURE</t>
   </si>
 </sst>
 </file>
@@ -429,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,10 +474,10 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -470,7 +497,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -490,7 +517,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -510,7 +537,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -530,13 +557,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -550,16 +577,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -570,16 +597,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -590,16 +617,76 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>